<commit_message>
olink prisming works for only study_npx
</commit_message>
<xml_diff>
--- a/template_examples/olink_template.xlsx
+++ b/template_examples/olink_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10115"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47A3941-C86F-E746-9198-7C15BD630CB8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4468D4-E181-694B-895D-4BD6DECEB805}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17820" yWindow="1420" windowWidth="20300" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="olink" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <author>CIDC</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{D2B0B813-F125-2548-8888-ECB169C12EFB}">
       <text>
         <r>
           <rPr>
@@ -38,7 +38,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{469A0A0C-3655-174A-9210-56C9BB0B32B4}">
       <text>
         <r>
           <rPr>
@@ -51,12 +51,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{13EB5F58-6F5B-0C43-B3A3-FDD559CF4102}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -64,25 +64,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{6F24E415-9A94-2A40-920E-6B70436A6172}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Type of file being uploaded</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -90,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{11306FA7-522C-4B42-95A7-66DB719B8B0A}">
       <text>
         <r>
           <rPr>
@@ -103,7 +90,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{973DD079-B71E-F34B-A08C-9C72391A5A36}">
       <text>
         <r>
           <rPr>
@@ -116,7 +103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{26E4C8BE-C185-074D-97D6-9576E910C5F4}">
       <text>
         <r>
           <rPr>
@@ -129,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{BC135B00-8EB0-A447-9007-86B1984491AC}">
       <text>
         <r>
           <rPr>
@@ -142,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{617EE495-57B5-7A45-B78B-2BA5C7270B47}">
       <text>
         <r>
           <rPr>
@@ -155,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{3316F90B-D448-1D4F-A419-F73AE9D58B20}">
       <text>
         <r>
           <rPr>
@@ -168,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+    <comment ref="J10" authorId="0" shapeId="0" xr:uid="{B9926783-DA7B-C344-8DA2-68D77C6F31D8}">
       <text>
         <r>
           <rPr>
@@ -181,12 +168,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="L6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
+    <comment ref="K10" authorId="0" shapeId="0" xr:uid="{92B12B9B-7AD4-364A-9BDD-CA52F40E9013}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -194,12 +181,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="M6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
+    <comment ref="L10" authorId="0" shapeId="0" xr:uid="{43C76271-3717-9B44-ABDD-17C41630A0CB}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -207,20 +194,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Panel used for the assay</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
+    <comment ref="M10" authorId="0" shapeId="0" xr:uid="{31C21D0C-652E-1245-8082-AF5563F9111D}">
       <text>
         <r>
           <rPr>
@@ -233,7 +207,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
+    <comment ref="N10" authorId="0" shapeId="0" xr:uid="{F38195E0-4D0A-A243-AFD2-97F8721C1024}">
       <text>
         <r>
           <rPr>
@@ -246,29 +220,16 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
+    <comment ref="O10" authorId="0" shapeId="0" xr:uid="{FE6BFC31-CA66-BF49-9C73-B496B70D6E36}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t>Version of NPX manager used for the analysis</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="R6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Lot Number of the assay panel</t>
         </r>
       </text>
     </comment>
@@ -277,7 +238,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="37">
   <si>
     <t>#t</t>
   </si>
@@ -294,6 +255,18 @@
     <t>ASSAY CREATOR</t>
   </si>
   <si>
+    <t>PANEL</t>
+  </si>
+  <si>
+    <t>ASSAY PANEL LOT</t>
+  </si>
+  <si>
+    <t>COMBINED FILE</t>
+  </si>
+  <si>
+    <t>COMBINED FILE NPX MANAGER VERSION</t>
+  </si>
+  <si>
     <t>Olink Assay details</t>
   </si>
   <si>
@@ -306,9 +279,6 @@
     <t>ASSAY_PREFIX</t>
   </si>
   <si>
-    <t>FILETYPE</t>
-  </si>
-  <si>
     <t>RUN DATE</t>
   </si>
   <si>
@@ -339,21 +309,21 @@
     <t>BASELINE CORRECTION</t>
   </si>
   <si>
-    <t>PANEL</t>
+    <t>NUMBER OF SAMPLES</t>
+  </si>
+  <si>
+    <t>NUMBER OF SAMPLES FAILED</t>
   </si>
   <si>
     <t>NPX MANAGER VERSION</t>
   </si>
   <si>
-    <t>ASSAY PANEL LOT</t>
+    <t>DFCI</t>
   </si>
   <si>
     <t>Olink_assay_1</t>
   </si>
   <si>
-    <t>assay</t>
-  </si>
-  <si>
     <t>MIOMARKHD411</t>
   </si>
   <si>
@@ -378,22 +348,7 @@
     <t>Olink_assay_2</t>
   </si>
   <si>
-    <t>Olink_assay_combined</t>
-  </si>
-  <si>
-    <t>study</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>DFCI</t>
-  </si>
-  <si>
-    <t>NUMBER OF SAMPLES</t>
-  </si>
-  <si>
-    <t>NUMBER OF SAMPLES FAILED</t>
+    <t>/local/path/combined.xlsx</t>
   </si>
 </sst>
 </file>
@@ -424,14 +379,14 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -461,7 +416,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -495,11 +450,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -507,11 +499,23 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -851,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R206"/>
+  <dimension ref="A1:Q210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -863,31 +867,30 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-    </row>
-    <row r="2" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+    </row>
+    <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -911,9 +914,8 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-    </row>
-    <row r="3" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -921,7 +923,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -937,1256 +939,1275 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B5" s="6" t="s">
+    </row>
+    <row r="4" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+    </row>
+    <row r="5" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+    </row>
+    <row r="6" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="1:17" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+    </row>
+    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q6" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R6" s="2" t="s">
+      <c r="L10" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="M10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="s">
+      <c r="N10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="4">
+      <c r="O10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="5">
         <v>43811</v>
       </c>
-      <c r="E7" s="5">
+      <c r="D11" s="6">
         <v>0.42430555555555555</v>
       </c>
-      <c r="F7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7">
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11">
         <v>20140305.43</v>
       </c>
-      <c r="I7">
+      <c r="H11">
         <v>13456777</v>
       </c>
-      <c r="J7" t="s">
-        <v>27</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="I11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11">
+        <v>0.5</v>
+      </c>
+      <c r="L11" t="s">
+        <v>32</v>
+      </c>
+      <c r="M11">
+        <v>90</v>
+      </c>
+      <c r="N11">
+        <v>5</v>
+      </c>
+      <c r="O11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="5">
+        <v>43811</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="E12" t="s">
         <v>28</v>
       </c>
-      <c r="L7">
+      <c r="F12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12">
+        <v>20140305.43</v>
+      </c>
+      <c r="H12">
+        <v>13456777</v>
+      </c>
+      <c r="I12" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K12">
         <v>0.5</v>
       </c>
-      <c r="M7" t="s">
-        <v>29</v>
-      </c>
-      <c r="N7" t="s">
-        <v>30</v>
-      </c>
-      <c r="O7">
-        <v>90</v>
-      </c>
-      <c r="P7">
-        <v>5</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>31</v>
-      </c>
-      <c r="R7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="L12" t="s">
         <v>32</v>
       </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="4">
-        <v>43811</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="F8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8">
-        <v>20140305.43</v>
-      </c>
-      <c r="I8">
-        <v>13456777</v>
-      </c>
-      <c r="J8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K8" t="s">
-        <v>28</v>
-      </c>
-      <c r="L8">
-        <v>0.5</v>
-      </c>
-      <c r="M8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N8" t="s">
-        <v>30</v>
-      </c>
-      <c r="O8">
+      <c r="M12">
         <v>80</v>
       </c>
-      <c r="P8">
+      <c r="N12">
         <v>10</v>
       </c>
-      <c r="Q8" t="s">
-        <v>31</v>
-      </c>
-      <c r="R8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="O12" t="s">
         <v>34</v>
       </c>
-      <c r="D9">
-        <v>43811</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="F9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" t="s">
-        <v>35</v>
-      </c>
-      <c r="H9" t="s">
-        <v>35</v>
-      </c>
-      <c r="I9" t="s">
-        <v>35</v>
-      </c>
-      <c r="J9" t="s">
-        <v>35</v>
-      </c>
-      <c r="K9" t="s">
-        <v>35</v>
-      </c>
-      <c r="L9" t="s">
-        <v>35</v>
-      </c>
-      <c r="M9" t="s">
-        <v>35</v>
-      </c>
-      <c r="N9" t="s">
-        <v>30</v>
-      </c>
-      <c r="O9">
-        <v>170</v>
-      </c>
-      <c r="P9">
-        <v>15</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>31</v>
-      </c>
-      <c r="R9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:R1"/>
-    <mergeCell ref="B5:R5"/>
+    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="B9:O9"/>
   </mergeCells>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{71FCE423-CB7D-684A-BC25-3FB6CBA1578C}">
       <formula1>"DFCI,Mount Sinai, Stanford, MD Anderson"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C206" xr:uid="{00000000-0002-0000-0000-000003000000}">
-      <formula1>"assay,study"</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="D7:D206" xr:uid="{00000000-0002-0000-0000-000004000000}">
-      <formula1>AND(ISNUMBER(D7:D206),LEFT(CELL("format",D7:D206),1)="D")</formula1>
-    </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="E10:E206 E7:E8" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="D11:D12" xr:uid="{BDEFDE59-F742-9C43-AFAB-0BF15DCB45FF}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C11:C12" xr:uid="{AD9CD908-0D70-114B-8B87-FE6338128C34}">
+      <formula1>AND(ISNUMBER(D11:D210),LEFT(CELL("format",D11:D210),1)="D")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
olink GCS filename collision / overwrite fixed
</commit_message>
<xml_diff>
--- a/template_examples/olink_template.xlsx
+++ b/template_examples/olink_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484E923E-5AFA-2B4B-BB0E-D16A691BDF12}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7BD2A8-F357-7D4E-93E8-B2625FEBBD90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7340" yWindow="960" windowWidth="20300" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{13EB5F58-6F5B-0C43-B3A3-FDD559CF4102}">
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{617EE495-57B5-7A45-B78B-2BA5C7270B47}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Chip barcode number</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{13EB5F58-6F5B-0C43-B3A3-FDD559CF4102}">
       <text>
         <r>
           <rPr>
@@ -64,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{4DC57F73-054D-6848-9835-CD754B758745}">
+    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{4DC57F73-054D-6848-9835-CD754B758745}">
       <text>
         <r>
           <rPr>
@@ -77,7 +90,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{6F24E415-9A94-2A40-920E-6B70436A6172}">
+    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{6F24E415-9A94-2A40-920E-6B70436A6172}">
       <text>
         <r>
           <rPr>
@@ -90,7 +103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{11306FA7-522C-4B42-95A7-66DB719B8B0A}">
+    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{11306FA7-522C-4B42-95A7-66DB719B8B0A}">
       <text>
         <r>
           <rPr>
@@ -103,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{973DD079-B71E-F34B-A08C-9C72391A5A36}">
+    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{973DD079-B71E-F34B-A08C-9C72391A5A36}">
       <text>
         <r>
           <rPr>
@@ -116,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{26E4C8BE-C185-074D-97D6-9576E910C5F4}">
+    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{26E4C8BE-C185-074D-97D6-9576E910C5F4}">
       <text>
         <r>
           <rPr>
@@ -129,29 +142,16 @@
         </r>
       </text>
     </comment>
-    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{BC135B00-8EB0-A447-9007-86B1984491AC}">
+    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{BC135B00-8EB0-A447-9007-86B1984491AC}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t>Build of the Fluidgm application used</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{617EE495-57B5-7A45-B78B-2BA5C7270B47}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Chip barcode number</t>
         </r>
       </text>
     </comment>
@@ -251,7 +251,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="39">
   <si>
     <t>#t</t>
   </si>
@@ -365,6 +365,9 @@
   </si>
   <si>
     <t>RAW CT FILE</t>
+  </si>
+  <si>
+    <t>test_prism_trial_id</t>
   </si>
 </sst>
 </file>
@@ -874,7 +877,7 @@
   <dimension ref="A1:Q210"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -883,7 +886,7 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -906,15 +909,15 @@
       <c r="P1" s="7"/>
       <c r="Q1" s="7"/>
     </row>
-    <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1">
-        <v>10021</v>
+      <c r="C2" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1081,28 +1084,28 @@
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>18</v>
@@ -1131,29 +1134,29 @@
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>26</v>
+      <c r="B11">
+        <v>1111</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="4">
         <v>43811</v>
       </c>
-      <c r="E11" s="5">
+      <c r="F11" s="5">
         <v>0.42430555555555555</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>27</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>28</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>20140305.43</v>
-      </c>
-      <c r="I11">
-        <v>13456777</v>
       </c>
       <c r="J11" t="s">
         <v>29</v>
@@ -1181,29 +1184,29 @@
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>34</v>
+      <c r="B12">
+        <v>1112</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="4">
         <v>43811</v>
       </c>
-      <c r="E12" s="5">
+      <c r="F12" s="5">
         <v>0.42430555555555555</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>27</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>28</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>20140305.43</v>
-      </c>
-      <c r="I12">
-        <v>13456777</v>
       </c>
       <c r="J12" t="s">
         <v>29</v>
@@ -2226,12 +2229,12 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{71FCE423-CB7D-684A-BC25-3FB6CBA1578C}">
       <formula1>"DFCI,Mount Sinai, Stanford, MD Anderson"</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="E11:E12" xr:uid="{BDEFDE59-F742-9C43-AFAB-0BF15DCB45FF}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="F11:F12" xr:uid="{BDEFDE59-F742-9C43-AFAB-0BF15DCB45FF}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="D11:D12" xr:uid="{AD9CD908-0D70-114B-8B87-FE6338128C34}">
-      <formula1>AND(ISNUMBER(D11:D210),LEFT(CELL("format",D11:D210),1)="D")</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="E11:E12" xr:uid="{AD9CD908-0D70-114B-8B87-FE6338128C34}">
+      <formula1>AND(ISNUMBER(D13:D210),LEFT(CELL("format",D13:D210),1)="D")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
olink template exmaple - removed empty column
</commit_message>
<xml_diff>
--- a/template_examples/olink_template.xlsx
+++ b/template_examples/olink_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7BD2A8-F357-7D4E-93E8-B2625FEBBD90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DEC5EA5-8068-1748-8361-BA3D079C489A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7340" yWindow="960" windowWidth="20300" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7340" yWindow="960" windowWidth="30860" windowHeight="18040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="olink" sheetId="1" r:id="rId1"/>
@@ -510,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -521,9 +521,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -874,42 +871,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q210"/>
+  <dimension ref="A1:P210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q1:Q1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="101" width="30.6640625" customWidth="1"/>
+    <col min="2" max="100" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-    </row>
-    <row r="2" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+    </row>
+    <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -932,9 +928,8 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-    </row>
-    <row r="3" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -957,9 +952,8 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -982,9 +976,8 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-    </row>
-    <row r="5" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1007,9 +1000,8 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-    </row>
-    <row r="6" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1032,9 +1024,8 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-    </row>
-    <row r="7" spans="1:17" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:16" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1057,29 +1048,27 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-    </row>
-    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="8" t="s">
+    </row>
+    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="6"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="9"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1128,9 +1117,8 @@
       <c r="P10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Q10" s="2"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1180,7 +1168,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1230,22 +1218,22 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -2222,7 +2210,7 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="B1:P1"/>
     <mergeCell ref="B9:P9"/>
   </mergeCells>
   <dataValidations count="3">

</xml_diff>

<commit_message>
update olink eg filenames
</commit_message>
<xml_diff>
--- a/template_examples/olink_template.xlsx
+++ b/template_examples/olink_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED9CFB7-D891-954A-BA17-4FCF05BC4564}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98DC8347-B3E8-B043-AD81-1967A5CE6624}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7340" yWindow="960" windowWidth="30860" windowHeight="18040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="21980" windowHeight="12800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="olink" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <author>CIDC</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{D2B0B813-F125-2548-8888-ECB169C12EFB}">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -34,11 +34,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Trial identifier used by lead organization, e.g. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
+          <t>Trial identifier used by lead organization, ie. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{469A0A0C-3655-174A-9210-56C9BB0B32B4}">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -47,11 +47,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Indicates what site is filling out the assay</t>
+          <t>Indicates what site is filling out the assay.</t>
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{617EE495-57B5-7A45-B78B-2BA5C7270B47}">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -60,11 +60,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Chip barcode number</t>
+          <t>Panel used for the assay.</t>
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{13EB5F58-6F5B-0C43-B3A3-FDD559CF4102}">
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lot number of the assay panel.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -73,11 +86,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Prefix to used for the filename</t>
+          <t>Combined file name on a user's computer.</t>
         </r>
       </text>
     </comment>
-    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{4DC57F73-054D-6848-9835-CD754B758745}">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -86,11 +99,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Prefix to used for the filename</t>
+          <t>Version of NPX manager used for the analysis.</t>
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{6F24E415-9A94-2A40-920E-6B70436A6172}">
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Chip barcode number.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -99,11 +125,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Date when the olink assay was run</t>
+          <t>NPX file name on a user's computer.</t>
         </r>
       </text>
     </comment>
-    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{11306FA7-522C-4B42-95A7-66DB719B8B0A}">
+    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -112,11 +138,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Time when the olink assay was run</t>
+          <t>Raw CT file name on a user's computer.</t>
         </r>
       </text>
     </comment>
-    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{973DD079-B71E-F34B-A08C-9C72391A5A36}">
+    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -125,11 +151,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Instrument used for the assay</t>
+          <t>Date when the Olink assay was run.</t>
         </r>
       </text>
     </comment>
-    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{26E4C8BE-C185-074D-97D6-9576E910C5F4}">
+    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -138,24 +164,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Version of the Fluidgm application used</t>
+          <t>Time when the Olink assay was run.</t>
         </r>
       </text>
     </comment>
-    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{BC135B00-8EB0-A447-9007-86B1984491AC}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Build of the Fluidgm application used</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J10" authorId="0" shapeId="0" xr:uid="{3316F90B-D448-1D4F-A419-F73AE9D58B20}">
+    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -164,11 +177,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Probe Type</t>
+          <t>Instrument used for the Olink assay.</t>
         </r>
       </text>
     </comment>
-    <comment ref="K10" authorId="0" shapeId="0" xr:uid="{B9926783-DA7B-C344-8DA2-68D77C6F31D8}">
+    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -177,72 +190,111 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Passive Reference</t>
+          <t>Version of the Fluidgm application used.</t>
         </r>
       </text>
     </comment>
-    <comment ref="L10" authorId="0" shapeId="0" xr:uid="{92B12B9B-7AD4-364A-9BDD-CA52F40E9013}">
+    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Threshold used for quality cutoff</t>
+          <t>Build of the Fluidgm application used.</t>
         </r>
       </text>
     </comment>
-    <comment ref="M10" authorId="0" shapeId="0" xr:uid="{43C76271-3717-9B44-ABDD-17C41630A0CB}">
+    <comment ref="J10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Method used for baseline correction</t>
+          <t>Probe Type.</t>
         </r>
       </text>
     </comment>
-    <comment ref="N10" authorId="0" shapeId="0" xr:uid="{31C21D0C-652E-1245-8082-AF5563F9111D}">
+    <comment ref="K10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Number of sample analyzed in the assay</t>
+          <t>Passive Reference.</t>
         </r>
       </text>
     </comment>
-    <comment ref="O10" authorId="0" shapeId="0" xr:uid="{F38195E0-4D0A-A243-AFD2-97F8721C1024}">
+    <comment ref="L10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Number of sample failed in the assay</t>
+          <t>Threshold used for quality cutoff.</t>
         </r>
       </text>
     </comment>
-    <comment ref="P10" authorId="0" shapeId="0" xr:uid="{FE6BFC31-CA66-BF49-9C73-B496B70D6E36}">
+    <comment ref="M10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Version of NPX manager used for the analysis</t>
+          <t>Method used for baseline correction.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of samples analyzed in the assay.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of samples failed in the assay.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Version of NPX manager used for the analysis.</t>
         </r>
       </text>
     </comment>
@@ -251,30 +303,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="41">
   <si>
     <t>#t</t>
   </si>
   <si>
-    <t>METADATA FILE FOR OLINK</t>
+    <t>Metadata file for olink</t>
   </si>
   <si>
     <t>#p</t>
   </si>
   <si>
-    <t>ASSAY CREATOR</t>
-  </si>
-  <si>
-    <t>PANEL</t>
-  </si>
-  <si>
-    <t>ASSAY PANEL LOT</t>
-  </si>
-  <si>
-    <t>COMBINED FILE</t>
-  </si>
-  <si>
-    <t>COMBINED FILE NPX MANAGER VERSION</t>
+    <t>Protocol identifier</t>
+  </si>
+  <si>
+    <t>Assay creator</t>
+  </si>
+  <si>
+    <t>Panel</t>
+  </si>
+  <si>
+    <t>Assay panel lot</t>
+  </si>
+  <si>
+    <t>Combined file</t>
+  </si>
+  <si>
+    <t>Combined file npx manager version</t>
   </si>
   <si>
     <t>Olink Assay details</t>
@@ -286,49 +341,64 @@
     <t>#d</t>
   </si>
   <si>
-    <t>RUN DATE</t>
-  </si>
-  <si>
-    <t>RUN TIME</t>
-  </si>
-  <si>
-    <t>INSTRUMENT</t>
-  </si>
-  <si>
-    <t>FLUDIGM APPLICATION VERSION</t>
-  </si>
-  <si>
-    <t>FLUDIGM APPLICATION BUILD</t>
-  </si>
-  <si>
-    <t>CHIP BARCODE</t>
-  </si>
-  <si>
-    <t>PROBE TYPE</t>
-  </si>
-  <si>
-    <t>PASSIVE REFERENCE</t>
-  </si>
-  <si>
-    <t>QUALITY THRESHOLD</t>
-  </si>
-  <si>
-    <t>BASELINE CORRECTION</t>
-  </si>
-  <si>
-    <t>NUMBER OF SAMPLES</t>
-  </si>
-  <si>
-    <t>NUMBER OF SAMPLES FAILED</t>
-  </si>
-  <si>
-    <t>NPX MANAGER VERSION</t>
+    <t>Chip barcode</t>
+  </si>
+  <si>
+    <t>Npx file</t>
+  </si>
+  <si>
+    <t>Raw ct file</t>
+  </si>
+  <si>
+    <t>Run date</t>
+  </si>
+  <si>
+    <t>Run time</t>
+  </si>
+  <si>
+    <t>Instrument</t>
+  </si>
+  <si>
+    <t>Fludigm application version</t>
+  </si>
+  <si>
+    <t>Fludigm application build</t>
+  </si>
+  <si>
+    <t>Probe type</t>
+  </si>
+  <si>
+    <t>Passive reference</t>
+  </si>
+  <si>
+    <t>Quality threshold</t>
+  </si>
+  <si>
+    <t>Baseline correction</t>
+  </si>
+  <si>
+    <t>Number of samples</t>
+  </si>
+  <si>
+    <t>Number of samples failed</t>
+  </si>
+  <si>
+    <t>Npx manager version</t>
+  </si>
+  <si>
+    <t>test_prism_trial_id</t>
   </si>
   <si>
     <t>DFCI</t>
   </si>
   <si>
-    <t>Olink_assay_1</t>
+    <t>Olink INFLAMMATION(v.3004)</t>
+  </si>
+  <si>
+    <t>Olink NPX Manager 0.0.82.0</t>
+  </si>
+  <si>
+    <t>olink_assay_combined.xlsx</t>
   </si>
   <si>
     <t>MIOMARKHD411</t>
@@ -346,28 +416,16 @@
     <t>Linear</t>
   </si>
   <si>
-    <t>Olink INFLAMMATION(v.3004)</t>
-  </si>
-  <si>
-    <t>Olink NPX Manager 0.0.82.0</t>
-  </si>
-  <si>
-    <t>Olink_assay_2</t>
-  </si>
-  <si>
-    <t>/local/path/combined.xlsx</t>
-  </si>
-  <si>
-    <t>NPX FILE</t>
-  </si>
-  <si>
-    <t>RAW CT FILE</t>
-  </si>
-  <si>
-    <t>test_prism_trial_id</t>
-  </si>
-  <si>
-    <t>PROTOCOL IDENTIFIER</t>
+    <t>olink_assay_1_NPX.xlsx</t>
+  </si>
+  <si>
+    <t>olink_assay_2_NPX.xlsx</t>
+  </si>
+  <si>
+    <t>olink_assay_1_CT.xlsx</t>
+  </si>
+  <si>
+    <t>olink_assay_2_CT.xlsx</t>
   </si>
 </sst>
 </file>
@@ -398,14 +456,14 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -435,7 +493,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -469,48 +527,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -518,20 +539,11 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -874,16 +886,16 @@
   <dimension ref="A1:P210"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="100" width="30.6640625" customWidth="1"/>
+    <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -905,15 +917,15 @@
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
     </row>
-    <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -929,15 +941,15 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -953,15 +965,15 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -977,12 +989,12 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -1001,15 +1013,15 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1025,15 +1037,15 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1049,87 +1061,87 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="9"/>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="G10" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>1111</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="E11" s="4">
         <v>43811</v>
@@ -1138,25 +1150,25 @@
         <v>0.42430555555555555</v>
       </c>
       <c r="G11" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="H11" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="I11">
         <v>20140305.43</v>
       </c>
       <c r="J11" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="K11" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="L11">
         <v>0.5</v>
       </c>
       <c r="M11" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="N11">
         <v>90</v>
@@ -1165,21 +1177,21 @@
         <v>5</v>
       </c>
       <c r="P11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>1112</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="E12" s="4">
         <v>43811</v>
@@ -1188,25 +1200,25 @@
         <v>0.42430555555555555</v>
       </c>
       <c r="G12" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="H12" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="I12">
         <v>20140305.43</v>
       </c>
       <c r="J12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="K12" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="L12">
         <v>0.5</v>
       </c>
       <c r="M12" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="N12">
         <v>80</v>
@@ -1215,997 +1227,997 @@
         <v>10</v>
       </c>
       <c r="P12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2213,15 +2225,18 @@
     <mergeCell ref="B1:P1"/>
     <mergeCell ref="B9:P9"/>
   </mergeCells>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{71FCE423-CB7D-684A-BC25-3FB6CBA1578C}">
-      <formula1>"DFCI,Mount Sinai, Stanford, MD Anderson"</formula1>
+  <dataValidations count="4">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="E13:E210" xr:uid="{00000000-0002-0000-0000-000001000000}">
+      <formula1>AND(ISNUMBER(E13:E212),LEFT(CELL("format",E13:E212),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="F11:F12" xr:uid="{BDEFDE59-F742-9C43-AFAB-0BF15DCB45FF}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="F11:F210" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="E11:E12" xr:uid="{AD9CD908-0D70-114B-8B87-FE6338128C34}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{831B46BC-225E-E54A-85EE-9A4A177D2436}">
+      <formula1>"DFCI,Mount Sinai, Stanford, MD Anderson"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="E11:E12" xr:uid="{A76CAE8A-6E0A-7346-9A35-A099D3E4458E}">
       <formula1>AND(ISNUMBER(D13:D210),LEFT(CELL("format",D13:D210),1)="D")</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
fix olink and other tests wrt prismify local_files extensions check
</commit_message>
<xml_diff>
--- a/template_examples/olink_template.xlsx
+++ b/template_examples/olink_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16684C0F-B17E-B341-B24D-496BDFD85AB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B45402-0B27-6C43-8F62-501C76EFA663}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="21980" windowHeight="12800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6200" yWindow="6260" windowWidth="21980" windowHeight="12800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="olink" sheetId="1" r:id="rId1"/>
@@ -419,13 +419,13 @@
     <t>olink_assay_2_NPX.xlsx</t>
   </si>
   <si>
-    <t>olink_assay_1_CT.xlsx</t>
-  </si>
-  <si>
-    <t>olink_assay_2_CT.xlsx</t>
-  </si>
-  <si>
     <t>test_prism_trial_id</t>
+  </si>
+  <si>
+    <t>olink_assay_1_CT.csv</t>
+  </si>
+  <si>
+    <t>olink_assay_2_CT.csv</t>
   </si>
 </sst>
 </file>
@@ -886,7 +886,7 @@
   <dimension ref="A1:P210"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -925,7 +925,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1141,7 +1141,7 @@
         <v>36</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E11" s="4">
         <v>43811</v>
@@ -1191,7 +1191,7 @@
         <v>37</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E12" s="4">
         <v>43811</v>

</xml_diff>

<commit_message>
Add test illustrating bug
</commit_message>
<xml_diff>
--- a/template_examples/olink_template.xlsx
+++ b/template_examples/olink_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlurye/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8A5230-39F9-4B41-A41E-F7102C224422}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8EC3A9-EF7A-A440-ADCA-029EBD3C6C81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -348,7 +348,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2141" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2143" uniqueCount="81">
   <si>
     <t>LEGEND</t>
   </si>
@@ -588,6 +588,9 @@
   </si>
   <si>
     <t>batch1</t>
+  </si>
+  <si>
+    <t>olink_assay_batch_combined.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1058,7 @@
   <dimension ref="A1:P2013"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1156,16 +1159,20 @@
       <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="C9" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>61</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="8" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">

</xml_diff>

<commit_message>
Fix typo in olink template merge pointer (#424)
* Add test illustrating bug

* Fix typo in merge pointer
</commit_message>
<xml_diff>
--- a/template_examples/olink_template.xlsx
+++ b/template_examples/olink_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlurye/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8A5230-39F9-4B41-A41E-F7102C224422}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8EC3A9-EF7A-A440-ADCA-029EBD3C6C81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -348,7 +348,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2141" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2143" uniqueCount="81">
   <si>
     <t>LEGEND</t>
   </si>
@@ -588,6 +588,9 @@
   </si>
   <si>
     <t>batch1</t>
+  </si>
+  <si>
+    <t>olink_assay_batch_combined.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1058,7 @@
   <dimension ref="A1:P2013"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1156,16 +1159,20 @@
       <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="C9" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>61</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="8" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">

</xml_diff>